<commit_message>
+ add max error acs759
</commit_message>
<xml_diff>
--- a/ACS759lcb-100U/ACS759lcb-100U.xlsx
+++ b/ACS759lcb-100U/ACS759lcb-100U.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chesi\Desktop\Git_Repo\DC_Load\HW\ACS759lcb-100U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C82E0E-CA7E-4FCF-B3F0-E3DC3AA20534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F81F3A6-D7AB-461A-AA33-A479CE9D2AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA8DAC84-6CD3-4DF4-B39D-0CFED206C9EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA8DAC84-6CD3-4DF4-B39D-0CFED206C9EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Current</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Errore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errore Max = </t>
   </si>
 </sst>
 </file>
@@ -52,12 +55,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +93,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -599,7 +627,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3033,25 +3060,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077BEA26-5745-462F-8BD1-BF929E01C473}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3359,8 +3386,23 @@
         <v>-34</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5">
+        <f>MIN(D2:D20)</f>
+        <v>-34</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A23:B23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>